<commit_message>
Desabilitar menu na tela inicial
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="402">
   <si>
     <t>nome aula</t>
   </si>
@@ -2059,6 +2059,15 @@
   </si>
   <si>
     <t>Navegação</t>
+  </si>
+  <si>
+    <t>2:12
+9. Aplicação Ionic - Parte 1/2
+116. Desabilitar menu na tela inicial
+eventos de ciclo de vida de uma página do Ionic - consultar documentação.. buscar por "ionic lifecycle events" no google. No caso vamos usar o "ionViewDidLoad" ... mas existem varios</t>
+  </si>
+  <si>
+    <t>Desabilitar menu na tela inicial</t>
   </si>
 </sst>
 </file>
@@ -2544,8 +2553,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F23" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F23"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7514,10 +7523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7929,6 +7938,24 @@
       </c>
       <c r="F22" s="19"/>
     </row>
+    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
+        <v>9</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C23" s="20">
+        <v>116</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="F23" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Obtendo os dados do formulario de login
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\JAVA\CURSO - SPRING BOOT, IONIC\FRONT-END\curso-spring-ionic-frontend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="421">
   <si>
     <t>nome aula</t>
   </si>
@@ -2156,6 +2156,27 @@
   </si>
   <si>
     <t>Mostrando as categorias</t>
+  </si>
+  <si>
+    <t>10:51
+9. Aplicação Ionic - Parte 1/2
+119. Criando um interceptor para tratamento de erros
+transfere a responsabilidade de captar o erros para a classe "error-interceptor.ts" imprimir na tela</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Criando um interceptor para tratamento de erros</t>
+  </si>
+  <si>
+    <t>2:08
+9. Aplicação Ionic - Parte 1/2
+120. Obtendo os dados do formulário de login
+combinação de binding de atributo de elemento HTML com binding de eventos para capturar valores de campos de texto da tela de login (usuario e senha).
+para binding de atributos usa-se "[ ]" abrir e fechar colchetes.
+para binding de eventos usa-se "( )" parenteses.
+como será uma combinação, usa-se: "[ ( ROTINA_AQUI ) ]"</t>
+  </si>
+  <si>
+    <t>Obtendo os dados do formulário de login</t>
   </si>
 </sst>
 </file>
@@ -2641,8 +2662,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F36" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F38" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F38"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7611,10 +7632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8280,6 +8301,42 @@
       </c>
       <c r="F36" s="19"/>
     </row>
+    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="20">
+        <v>9</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C37" s="20">
+        <v>119</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>417</v>
+      </c>
+      <c r="F37" s="19"/>
+    </row>
+    <row r="38" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+      <c r="A38" s="20">
+        <v>9</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C38" s="20">
+        <v>120</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="F38" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Comecando a implementar a autenticacao
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="423">
   <si>
     <t>nome aula</t>
   </si>
@@ -2177,6 +2177,15 @@
   </si>
   <si>
     <t>Obtendo os dados do formulário de login</t>
+  </si>
+  <si>
+    <t>5:18
+9. Aplicação Ionic - Parte 1/2
+121. Começando a implementar a autenticação
+lembrar sempre de declarar as novas classes em app.module.ts ... nos providers. Neste caso a classe criada auth.service.ts, para que tenhamos uma instancia do serviço disponivel na aplicação.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Começando a implementar a autenticação</t>
   </si>
 </sst>
 </file>
@@ -2662,8 +2671,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F38" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F39" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F39"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7632,10 +7641,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8337,6 +8346,24 @@
       </c>
       <c r="F38" s="19"/>
     </row>
+    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="20">
+        <v>9</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C39" s="20">
+        <v>121</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>422</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>421</v>
+      </c>
+      <c r="F39" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Salvando os dados do usuario logado no localStorage
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="425">
   <si>
     <t>nome aula</t>
   </si>
@@ -2186,6 +2186,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Começando a implementar a autenticação</t>
+  </si>
+  <si>
+    <t>0:18
+9. Aplicação Ionic - Parte 1/2
+122. Salvando os dados do usuário logado no localStorage
+localStorage: é uma propriedade de armazenamento local que veio com o HTML5 que tem a função de armazenar strings na forma de par chave/valor</t>
+  </si>
+  <si>
+    <t>Salvando os dados do usuário logado no localStorage</t>
   </si>
 </sst>
 </file>
@@ -2671,8 +2680,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F39" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F40" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F40"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7641,10 +7650,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8364,6 +8373,24 @@
       </c>
       <c r="F39" s="19"/>
     </row>
+    <row r="40" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="20">
+        <v>9</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C40" s="20">
+        <v>122</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>423</v>
+      </c>
+      <c r="F40" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Extraindo o email do token e armazendno-o em localStorage
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="428">
   <si>
     <t>nome aula</t>
   </si>
@@ -2195,6 +2195,25 @@
   </si>
   <si>
     <t>Salvando os dados do usuário logado no localStorage</t>
+  </si>
+  <si>
+    <t>0:31
+9. Aplicação Ionic - Parte 1/2
+123. Extraindo o email do token e armazenando-o em localStorage
+necessário instalar dependência com o comando "npm install --save angular2-jwt" para manipular token jwt</t>
+  </si>
+  <si>
+    <t>2:51
+9. Aplicação Ionic - Parte 1/2
+123. Extraindo o email do token e armazenando-o em localStorage
+no teste da aula, gera um erro no /node_modules/angular2-jwt/angular2-jwt.d.ts.
+para resolver, foi utilizado a sugestão do aluno nos comentarios da aula que foi a seguinte;
+fonte:
+https://stackoverflow.com/questions/38510369/cannot-find-module-angular-http
+Rodar o comando "npm install @angular/http@latest" no terminal na pasta do projeto</t>
+  </si>
+  <si>
+    <t>Extraindo o email do token e armazenando-o em localStorage</t>
   </si>
 </sst>
 </file>
@@ -2680,8 +2699,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F40" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F42" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F42"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7650,10 +7669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8391,6 +8410,42 @@
       </c>
       <c r="F40" s="19"/>
     </row>
+    <row r="41" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="20">
+        <v>9</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C41" s="20">
+        <v>123</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="F41" s="19"/>
+    </row>
+    <row r="42" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A42" s="20">
+        <v>9</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C42" s="20">
+        <v>123</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>426</v>
+      </c>
+      <c r="F42" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Criando uma pagina de profile
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="431">
   <si>
     <t>nome aula</t>
   </si>
@@ -2214,6 +2214,21 @@
   </si>
   <si>
     <t>Extraindo o email do token e armazenando-o em localStorage</t>
+  </si>
+  <si>
+    <t>0:18
+9. Aplicação Ionic - Parte 1/2
+124. Criando uma página de profile
+criação da pagina de profile com o comando "ionic generate page profile"</t>
+  </si>
+  <si>
+    <t>2:37
+9. Aplicação Ionic - Parte 1/2
+124. Criando uma página de profile
+acrescentando itens na pagina de menu: Categoria e Profile</t>
+  </si>
+  <si>
+    <t>Criando uma página de profile</t>
   </si>
 </sst>
 </file>
@@ -2699,8 +2714,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F42" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F44" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F44"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7669,10 +7684,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8446,6 +8461,44 @@
       </c>
       <c r="F42" s="19"/>
     </row>
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="20">
+        <v>9</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C43" s="20">
+        <v>124</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="20">
+        <v>9</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C44" s="20">
+        <v>124</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="F44" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Mostrando dados e imagem do cliente para pagina de profile
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="436">
   <si>
     <t>nome aula</t>
   </si>
@@ -2229,6 +2229,33 @@
   </si>
   <si>
     <t>Criando uma página de profile</t>
+  </si>
+  <si>
+    <t>2:15
+9. Aplicação Ionic - Parte 1/2
+125. Mostrando dados e imagem do cliente para página de profile
+em TypeScript, para colocar um atribbuto como OPCIONAL basta inserir o caracteres de interrogação "?" na frente dele. Ex.: email?: string;</t>
+  </si>
+  <si>
+    <t>7:52
+9. Aplicação Ionic - Parte 1/2
+125. Mostrando dados e imagem do cliente para página de profile
+lembrar sempre de registrar services em app.module.ts</t>
+  </si>
+  <si>
+    <t>10:59
+9. Aplicação Ionic - Parte 1/2
+125. Mostrando dados e imagem do cliente para página de profile
+[src] - source entre colchetes significa que é um binding de dados</t>
+  </si>
+  <si>
+    <t>11:31
+9. Aplicação Ionic - Parte 1/2
+125. Mostrando dados e imagem do cliente para página de profile
+ja no caso do angular, o operador "?" é o operador de navegação segura do angular.Significa que se a varável não tiver nenhum valor, não causará um erro na página.</t>
+  </si>
+  <si>
+    <t>Mostrando dados e imagem do cliente para página de profile</t>
   </si>
 </sst>
 </file>
@@ -2714,8 +2741,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F44" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F48" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F48"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7684,10 +7711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8499,6 +8526,80 @@
       </c>
       <c r="F44" s="19"/>
     </row>
+    <row r="45" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="20">
+        <v>9</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C45" s="20">
+        <v>125</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="20">
+        <v>9</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C46" s="20">
+        <v>125</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>432</v>
+      </c>
+      <c r="F46" s="19"/>
+    </row>
+    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="20">
+        <v>9</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C47" s="20">
+        <v>125</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>433</v>
+      </c>
+      <c r="F47" s="19"/>
+    </row>
+    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="20">
+        <v>9</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C48" s="20">
+        <v>125</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="F48" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Interceptor para incluir token nas requisições
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\JAVA\CURSO - SPRING BOOT, IONIC\FRONT-END\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="441">
   <si>
     <t>nome aula</t>
   </si>
@@ -2256,6 +2256,33 @@
   </si>
   <si>
     <t>Mostrando dados e imagem do cliente para página de profile</t>
+  </si>
+  <si>
+    <t>0:26
+9. Aplicação Ionic - Parte 1/2
+126. Interceptor para incluir token nas requisições
+links de referências da aula - para ler!</t>
+  </si>
+  <si>
+    <t>4:49
+9. Aplicação Ionic - Parte 1/2
+126. Interceptor para incluir token nas requisições
+ordem de execução dos providers: neste caso foi registrado o AuthInterceptorProvider para ser executado antes do ErrorInterceptorProvider. Para alterar a ordem de execução dos providers basta altera-los na classe pincipal "app.module.ts"</t>
+  </si>
+  <si>
+    <t>5:48
+9. Aplicação Ionic - Parte 1/2
+126. Interceptor para incluir token nas requisições
+IMPORTANTE: criação de código para não enviar header "Authorization" em caso de requisição para o bucket do S3 - enviar somente caso a requisição seja para a aplicação do STS ... como se fosse autorizado somente enviar o header para o ambiente de dev/test</t>
+  </si>
+  <si>
+    <t>6:27
+9. Aplicação Ionic - Parte 1/2
+126. Interceptor para incluir token nas requisições
+ótima dica para comparar a string da URL - estudo de caso para comparação de URL - testa a string URL da requisição</t>
+  </si>
+  <si>
+    <t>Interceptor para incluir token nas requisições</t>
   </si>
 </sst>
 </file>
@@ -2741,8 +2768,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F48" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F52" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F52"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7711,10 +7738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8600,6 +8627,78 @@
       </c>
       <c r="F48" s="19"/>
     </row>
+    <row r="49" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="20">
+        <v>9</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C49" s="20">
+        <v>126</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="F49" s="19"/>
+    </row>
+    <row r="50" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A50" s="20">
+        <v>9</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C50" s="20">
+        <v>126</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="F50" s="19"/>
+    </row>
+    <row r="51" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A51" s="20">
+        <v>9</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C51" s="20">
+        <v>126</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>438</v>
+      </c>
+      <c r="F51" s="19"/>
+    </row>
+    <row r="52" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="20">
+        <v>9</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C52" s="20">
+        <v>126</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="F52" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Tratamento padrao para outros erros com Alert
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\JAVA\CURSO - SPRING BOOT, IONIC\FRONT-END\curso-spring-ionic-frontend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="445">
   <si>
     <t>nome aula</t>
   </si>
@@ -2292,6 +2292,15 @@
   </si>
   <si>
     <t>Tratando erros 403</t>
+  </si>
+  <si>
+    <t>2:53
+9. Aplicação Ionic - Parte 1/2
+128. Tratamento padrão para outros erros com Alert
+uso de "alert" no ionic: ele funciona como o msgbox do VBA ou o JOptionPane. Uma propriedade interessante de configuração mostrada na aula é a propriedade "enableBackDropDismiss", que é um booleano onde permite o usuario tocar fora do alert para sair do mesmo ou obriga ele a apertar no botão designado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tratamento padrão para outros erros com Alert</t>
   </si>
 </sst>
 </file>
@@ -2777,8 +2786,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F53" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F54" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F54"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7747,10 +7756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8726,6 +8735,24 @@
       </c>
       <c r="F53" s="19"/>
     </row>
+    <row r="54" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="20">
+        <v>9</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C54" s="20">
+        <v>128</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="F54" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fazendo o app aproveitar o usuario logado na tela inicial
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="447">
   <si>
     <t>nome aula</t>
   </si>
@@ -2301,6 +2301,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Tratamento padrão para outros erros com Alert</t>
+  </si>
+  <si>
+    <t>3:20
+9. Aplicação Ionic - Parte 1/2
+129. Fazendo o app aproveitar o usuário logado na tela inicial
+nesta aula foi implementado o reuso de token ... onde caso o token do usuario esteja valido, a aplicação inicia direto na pagina de categorias invés da pagina de login</t>
+  </si>
+  <si>
+    <t>Fazendo o app aproveitar o usuário logado na tela inicial</t>
   </si>
 </sst>
 </file>
@@ -2786,8 +2795,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F54" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F55" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F55"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7756,10 +7765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8753,6 +8762,24 @@
       </c>
       <c r="F54" s="19"/>
     </row>
+    <row r="55" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A55" s="20">
+        <v>9</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C55" s="20">
+        <v>129</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="F55" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Criando um FormGroup para controlar o formulario
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\JAVA\CURSO - SPRING BOOT, IONIC\FRONT-END\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="453">
   <si>
     <t>nome aula</t>
   </si>
@@ -2310,6 +2310,39 @@
   </si>
   <si>
     <t>Fazendo o app aproveitar o usuário logado na tela inicial</t>
+  </si>
+  <si>
+    <t>0:09
+9. Aplicação Ionic - Parte 1/2
+132. Criando um FormGroup para controlar o formulário
+criação de FormGroup: FormGroup é um objeto do Angular React Forms - ajuda a controlar forms e fazer validações de forma interessante</t>
+  </si>
+  <si>
+    <t>3:19
+9. Aplicação Ionic - Parte 1/2
+132. Criando um FormGroup para controlar o formulário
+validações de campos no angular - usando o Validators na pagina de signup</t>
+  </si>
+  <si>
+    <t>4:34
+9. Aplicação Ionic - Parte 1/2
+132. Criando um FormGroup para controlar o formulário
+mostra uma forma de deixar devidamente preenchido campos de formulario (para testes) com o formGroup e o formBuilder</t>
+  </si>
+  <si>
+    <t>6:02
+9. Aplicação Ionic - Parte 1/2
+132. Criando um FormGroup para controlar o formulário
+ensina a fazer um binding dos elementos de um formGroup no arquivo typescript .ts ligando aos elementos do formulario HTML</t>
+  </si>
+  <si>
+    <t>6:33
+9. Aplicação Ionic - Parte 1/2
+132. Criando um FormGroup para controlar o formulário
+IMPORTANTE: para ligar o formGroup do arquivo .ts com o arquivo HTML é necessário fazer um BINDING DE ATRIBUTO ligando uma variavel local do HTML com a variavel do arquivo .ts - os nomes de variáveis devem coincidir</t>
+  </si>
+  <si>
+    <t>Criando um FormGroup para controlar o formulário</t>
   </si>
 </sst>
 </file>
@@ -2795,8 +2828,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F55" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F60" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F60"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7765,10 +7798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8780,6 +8813,96 @@
       </c>
       <c r="F55" s="19"/>
     </row>
+    <row r="56" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="20">
+        <v>9</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C56" s="20">
+        <v>132</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>447</v>
+      </c>
+      <c r="F56" s="19"/>
+    </row>
+    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="20">
+        <v>9</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C57" s="20">
+        <v>132</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="F57" s="19"/>
+    </row>
+    <row r="58" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A58" s="20">
+        <v>9</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C58" s="20">
+        <v>132</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="F58" s="19"/>
+    </row>
+    <row r="59" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A59" s="20">
+        <v>9</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C59" s="20">
+        <v>132</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="F59" s="19"/>
+    </row>
+    <row r="60" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A60" s="20">
+        <v>9</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C60" s="20">
+        <v>132</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>451</v>
+      </c>
+      <c r="F60" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Povoando dinamicamente estado e cidade
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\CURSO - SPRING BOOT, IONIC\ws-ionic\cursoSpringIonic\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="455">
   <si>
     <t>nome aula</t>
   </si>
@@ -2343,6 +2343,15 @@
   </si>
   <si>
     <t>Criando um FormGroup para controlar o formulário</t>
+  </si>
+  <si>
+    <t>11:04
+9. Aplicação Ionic - Parte 1/2
+133. Povoando dinamicamente estado e cidade
+neste trecho conhecemos o evento de seleção de item na combobox, o (ionChange)="" ... como em sistemas desktop, executa uma ação sempre que for selecionado um item... no caso, a combobox é de seleção de Estados e ao ser selecionado um estado, ativa o evento para listar e popular a combobox seguinte de Cidades</t>
+  </si>
+  <si>
+    <t>Povoando dinamicamente estado e cidade</t>
   </si>
 </sst>
 </file>
@@ -2828,8 +2837,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F60" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F61" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F61"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7798,10 +7807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8903,6 +8912,24 @@
       </c>
       <c r="F60" s="19"/>
     </row>
+    <row r="61" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A61" s="20">
+        <v>9</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C61" s="20">
+        <v>133</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>453</v>
+      </c>
+      <c r="F61" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Carregando produtos de uma dada categoria
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="462">
   <si>
     <t>nome aula</t>
   </si>
@@ -2368,6 +2368,28 @@
   </si>
   <si>
     <t>Salvando novo cliente</t>
+  </si>
+  <si>
+    <t>2:29
+9. Aplicação Ionic - Parte 1/2
+137. Carregando produtos de uma dada categoria
+IMPORTANTE:  primeira navegação entre paginas (push), passando parametros de uma página para outra</t>
+  </si>
+  <si>
+    <t>3:16
+9. Aplicação Ionic - Parte 1/2
+137. Carregando produtos de uma dada categoria
+para enviar parametros de uma pagina para outra seja ele no push ou no setRoot, basta incluir mais um parametro no metodo push/setRoot e colocar estes dados dentro de chaves { } em forma de objeto
+Ex.: this.navCtrl.push('ProdutosPage',{cat_id: categoria_id })</t>
+  </si>
+  <si>
+    <t>6:17
+9. Aplicação Ionic - Parte 1/2
+137. Carregando produtos de uma dada categoria
+para pegar o valor de um parametro passado por outra pagina (na pagina recebedora) é utilizado o NavParams</t>
+  </si>
+  <si>
+    <t>Carregando produtos de uma dada categoria</t>
   </si>
 </sst>
 </file>
@@ -2853,8 +2875,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F63" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F66" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F66"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7823,10 +7845,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8984,6 +9006,60 @@
       </c>
       <c r="F63" s="19"/>
     </row>
+    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A64" s="20">
+        <v>9</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C64" s="20">
+        <v>137</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>458</v>
+      </c>
+      <c r="F64" s="19"/>
+    </row>
+    <row r="65" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A65" s="20">
+        <v>9</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C65" s="20">
+        <v>137</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>459</v>
+      </c>
+      <c r="F65" s="19"/>
+    </row>
+    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="20">
+        <v>9</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C66" s="20">
+        <v>137</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="F66" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Carregando dados do produto
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="464">
   <si>
     <t>nome aula</t>
   </si>
@@ -2390,6 +2390,18 @@
   </si>
   <si>
     <t>Carregando produtos de uma dada categoria</t>
+  </si>
+  <si>
+    <t>0:29
+9. Aplicação Ionic - Parte 1/2
+140. Carregando dados do produto
+ProdutoService - inclusão dos métodos findById e getImageFromBucket
+produtos.ts - inclusão de parametro id no metodo showDetail na chamada de push
+produtos.html - inclusao do id do produto como parametro da chamada do metodo showDetail
+produto-detail.ts, fazer alterações necessarias</t>
+  </si>
+  <si>
+    <t>Carregando dados do produto</t>
   </si>
 </sst>
 </file>
@@ -2875,8 +2887,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F66" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F67" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F67"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7845,10 +7857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9060,6 +9072,24 @@
       </c>
       <c r="F66" s="19"/>
     </row>
+    <row r="67" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A67" s="20">
+        <v>9</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C67" s="20">
+        <v>140</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="F67" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Criando pagina de carrinho de compras
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\JAVA\CURSO - SPRING BOOT, IONIC\FRONT-END\curso-spring-ionic-frontend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="466">
   <si>
     <t>nome aula</t>
   </si>
@@ -2402,6 +2402,15 @@
   </si>
   <si>
     <t>Carregando dados do produto</t>
+  </si>
+  <si>
+    <t>18:49
+9. Aplicação Ionic - Parte 1/2
+141. Criando página de carrinho de compras
+implementado a pagina de carrinho ...rota categorias ... seleciona categoriaa ... depois seleciona o produto ... vai para a pagina de detalhes do produto ... clica em adicionar ao carrinho e enfim, mostra a pagina de carrinho com o produto adicionado</t>
+  </si>
+  <si>
+    <t>Criando página de carrinho de compras</t>
   </si>
 </sst>
 </file>
@@ -2887,8 +2896,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F67" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F68" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7857,10 +7866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9090,6 +9099,24 @@
       </c>
       <c r="F67" s="19"/>
     </row>
+    <row r="68" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A68" s="20">
+        <v>9</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C68" s="20">
+        <v>141</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>465</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="F68" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Acesso ao carrinho: botao flutuante e menu
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\JAVA\CURSO - SPRING BOOT, IONIC\FRONT-END\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="468">
   <si>
     <t>nome aula</t>
   </si>
@@ -2411,6 +2411,15 @@
   </si>
   <si>
     <t>Criando página de carrinho de compras</t>
+  </si>
+  <si>
+    <t>Acesso ao carrinho: botão flutuante e menu</t>
+  </si>
+  <si>
+    <t>1:57
+9. Aplicação Ionic - Parte 1/2
+143. Acesso ao carrinho: botão flutuante e menu
+INTERESSANTE: botão flutuante de navegação diretamente na tag HTML (navPush) invés de ser no typescript</t>
   </si>
 </sst>
 </file>
@@ -2896,8 +2905,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F68" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F69" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F69"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7866,10 +7875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9117,6 +9126,24 @@
       </c>
       <c r="F68" s="19"/>
     </row>
+    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="20">
+        <v>9</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C69" s="20">
+        <v>143</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>466</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="F69" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Tela de escolha de endereco
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\CURSO - SPRING BOOT, IONIC\ws-ionic\curso-spring-ionic-frontend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="471">
   <si>
     <t>nome aula</t>
   </si>
@@ -2420,6 +2420,18 @@
 9. Aplicação Ionic - Parte 1/2
 143. Acesso ao carrinho: botão flutuante e menu
 INTERESSANTE: botão flutuante de navegação diretamente na tag HTML (navPush) invés de ser no typescript</t>
+  </si>
+  <si>
+    <t>6:19
+10. Aplicação Ionic - Parte 2/2
+146. Tela de escolha de endereço
+INTERESSANTE: nesta aula, na criação do HTML da pagina PickAdress, esta sendo utizilizado tags H2 e P sendo que o preenchimento dela esta sendo com mais de um argumento do backend em uma unica tag usando concatenação</t>
+  </si>
+  <si>
+    <t>Tela de escolha de endereço</t>
+  </si>
+  <si>
+    <t>Aplicação Ionic - Parte 2/2</t>
   </si>
 </sst>
 </file>
@@ -2905,8 +2917,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F69" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F70" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F70"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7875,10 +7887,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:P70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9144,6 +9156,24 @@
       </c>
       <c r="F69" s="19"/>
     </row>
+    <row r="70" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="20">
+        <v>10</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C70" s="20">
+        <v>146</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>468</v>
+      </c>
+      <c r="F70" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Buscando enderecos do banco de dados
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\CURSO - SPRING BOOT, IONIC\ws-ionic\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="474">
   <si>
     <t>nome aula</t>
   </si>
@@ -2432,6 +2432,22 @@
   </si>
   <si>
     <t>Aplicação Ionic - Parte 2/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1:23
+10. Aplicação Ionic - Parte 2/2
+147. Buscando endereços do banco de dados
+alteração do metodo findByEmail da classe ClienteService; foi removido a TIPAGEM do tipo ClienteDTO pois aqui no front-end, ClienteDTO retorna somente id, nome, email e imagem ao retirar a tipagem, sera retornado o objeto inteiro do BACK-END, inclusive os endereços associados do cliente</t>
+  </si>
+  <si>
+    <t>2:56
+10. Aplicação Ionic - Parte 2/2
+147. Buscando endereços do banco de dados
+primeiro uso de CASTING no typescript, tornando um Cliente em ClienteDTO na classe ProfilePage no metodo ionViewDidLoad. Importante lembrar que, no frontend não possui uma classe existente da entidade Cliente... porém, o Cliente possui os dados que ClienteDTO (com classe existente no frontend) também possui, o que permite o casting</t>
+  </si>
+  <si>
+    <t>Buscando endereços do banco de dados</t>
   </si>
 </sst>
 </file>
@@ -2917,8 +2933,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F70" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F72" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F72"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7887,10 +7903,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P70"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9174,6 +9190,42 @@
       </c>
       <c r="F70" s="19"/>
     </row>
+    <row r="71" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A71" s="20">
+        <v>10</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C71" s="20">
+        <v>147</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>471</v>
+      </c>
+      <c r="F71" s="19"/>
+    </row>
+    <row r="72" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A72" s="20">
+        <v>10</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C72" s="20">
+        <v>147</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="E72" s="20" t="s">
+        <v>472</v>
+      </c>
+      <c r="F72" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Armazenamento dos dados do pedido
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="478">
   <si>
     <t>nome aula</t>
   </si>
@@ -2448,6 +2448,24 @@
   </si>
   <si>
     <t>Buscando endereços do banco de dados</t>
+  </si>
+  <si>
+    <t>3:20
+10. Aplicação Ionic - Parte 2/2
+148. Armazenamento dos dados do pedido
+para o @type - que é o tipo de pagamento, o typescript não permite colocar diretamente o caractere @ ... para usa-lo é necessário utilizar dentro de aspas "@type".</t>
+  </si>
+  <si>
+    <t>18:29
+10. Aplicação Ionic - Parte 2/2
+148. Armazenamento dos dados do pedido
+neste video aprendido algo muito interessante; como captar dados de objetos por partes (primeiro cliente, depois endereço de entrega e depois os itens do pedido) e somente inseri-los no banco de dados na finalização de um pedido. um ótimo exemplo para captar dados entre varias paginas e ao final, inserir no banco tudo de uma vez só.</t>
+  </si>
+  <si>
+    <t>Armazenamento dos dados do pedido</t>
+  </si>
+  <si>
+    <t>IMPORTANTE</t>
   </si>
 </sst>
 </file>
@@ -2933,8 +2951,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F72" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F74" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F74"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7903,10 +7921,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9226,6 +9244,46 @@
       </c>
       <c r="F72" s="19"/>
     </row>
+    <row r="73" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A73" s="20">
+        <v>10</v>
+      </c>
+      <c r="B73" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C73" s="20">
+        <v>148</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>476</v>
+      </c>
+      <c r="E73" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A74" s="20">
+        <v>10</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C74" s="20">
+        <v>148</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>476</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>475</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>477</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Tela de escolha de pagamento
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="480">
   <si>
     <t>nome aula</t>
   </si>
@@ -2467,6 +2467,15 @@
   <si>
     <t>IMPORTANTE</t>
   </si>
+  <si>
+    <t>10:17
+10. Aplicação Ionic - Parte 2/2
+149. Tela de escolha de pagamento
+trafegando os dados de um pedido via parametros entre telas - da tela de endereço para a tela de pagamento - e na próxima aula sera da tela de pagamento para tela de confirmação de pedido</t>
+  </si>
+  <si>
+    <t>Tela de escolha de pagamento</t>
+  </si>
 </sst>
 </file>
 
@@ -2574,7 +2583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2628,6 +2637,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2951,8 +2961,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F74" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F75" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F75"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7921,10 +7931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9284,9 +9294,32 @@
         <v>477</v>
       </c>
     </row>
+    <row r="75" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A75" s="20">
+        <v>10</v>
+      </c>
+      <c r="B75" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C75" s="20">
+        <v>149</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>479</v>
+      </c>
+      <c r="E75" s="20" t="s">
+        <v>478</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Usando Cordova para tirar foto com a camera
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\front-end\curso-spring-ionic-frontend\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\JAVA\CURSO - SPRING BOOT, IONIC\FRONT-END\curso-spring-ionic-frontend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="487">
   <si>
     <t>nome aula</t>
   </si>
@@ -2485,12 +2485,88 @@
   <si>
     <t>Infinite Scroll</t>
   </si>
+  <si>
+    <t>1:05
+10. Aplicação Ionic - Parte 2/2
+156. Usando Cordova para tirar foto com a câmera
+ensina a utilizar camera para tirar foto no ionic/cordova com o comando "ionic cordova platform add browser --save" ... neste caso foi adicionado como plataforma o próprio browser .. mas poderia ser android ou ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+2:42
+10. Aplicação Ionic - Parte 2/2
+156. Usando Cordova para tirar foto com a câmera
+instala plugin da camera com o comando "ionic cordova plugin add cordova-plugin-camera"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2:44
+10. Aplicação Ionic - Parte 2/2
+156. Usando Cordova para tirar foto com a câmera
+instala outro plugin da camera com o comando "npm install --save @ionic-native/camera" (NÃO FUNCIONA)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>edit: devido ao conflito de versões, executar o comando "npm install --save @ionic-native/camera@4.5.3"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3:43
+10. Aplicação Ionic - Parte 2/2
+156. Usando Cordova para tirar foto com a câmera
+comando</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> "ionic serve" não funciona mais</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> devido o serviço nativo cordova com camera
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+é necessário usar o comando "ionic cordova run browser"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Usando Cordova para tirar foto com a câmera</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2568,6 +2644,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -2972,8 +3064,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F76" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F80" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F80"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -7942,10 +8034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9343,6 +9435,78 @@
       </c>
       <c r="F76" s="21"/>
     </row>
+    <row r="77" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>10</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C77" s="20">
+        <v>156</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>486</v>
+      </c>
+      <c r="E77" s="20" t="s">
+        <v>482</v>
+      </c>
+      <c r="F77" s="19"/>
+    </row>
+    <row r="78" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>10</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C78" s="20">
+        <v>156</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>486</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="F78" s="19"/>
+    </row>
+    <row r="79" spans="1:6" ht="151.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="20">
+        <v>10</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C79" s="20">
+        <v>156</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>486</v>
+      </c>
+      <c r="E79" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="F79" s="19"/>
+    </row>
+    <row r="80" spans="1:6" ht="117" x14ac:dyDescent="0.45">
+      <c r="A80" s="20">
+        <v>10</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C80" s="18">
+        <v>156</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>486</v>
+      </c>
+      <c r="E80" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="F80" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fazendo upload da foto
</commit_message>
<xml_diff>
--- a/temp/anotacoes.xlsx
+++ b/temp/anotacoes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="489">
   <si>
     <t>nome aula</t>
   </si>
@@ -2560,6 +2560,16 @@
   </si>
   <si>
     <t xml:space="preserve"> Usando Cordova para tirar foto com a câmera</t>
+  </si>
+  <si>
+    <t>0:33
+10. Aplicação Ionic - Parte 2/2
+157. Fazendo upload da foto
+referencia de como converter a imagem em formato base64 pra blob pois no backend é usado o tipo blob
+https://gist.github.com/fupslot/5015897</t>
+  </si>
+  <si>
+    <t>Fazendo upload da foto</t>
   </si>
 </sst>
 </file>
@@ -3064,8 +3074,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F80" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F81" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F81"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Seção" dataDxfId="5"/>
     <tableColumn id="2" name="Nome da Seção" dataDxfId="4"/>
@@ -8034,10 +8044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9507,6 +9517,24 @@
       </c>
       <c r="F80" s="19"/>
     </row>
+    <row r="81" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>10</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C81" s="20">
+        <v>157</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>488</v>
+      </c>
+      <c r="E81" s="20" t="s">
+        <v>487</v>
+      </c>
+      <c r="F81" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>